<commit_message>
[Update] Radiation impedance calculation using HKI_Sub_Integral_Ls_theta (Single FFR) - Divide 9 ranages and Ls_theta integration
</commit_message>
<xml_diff>
--- a/1. Arbitrary Array (3,4Array)/Single_FFR_Relative_Error - 과거 HKI 버젼.xlsx
+++ b/1. Arbitrary Array (3,4Array)/Single_FFR_Relative_Error - 과거 HKI 버젼.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="45" documentId="6_{3952EC13-6099-488B-A735-225E12CBDEC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{73A85804-8FB9-4966-8A85-FEB1E29A368E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="17385" activeTab="3" xr2:uid="{F809ED7E-B7F2-4D14-9E2F-854BB1B1388F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="17385" xr2:uid="{F809ED7E-B7F2-4D14-9E2F-854BB1B1388F}"/>
   </bookViews>
   <sheets>
     <sheet name="Z_11" sheetId="1" r:id="rId1"/>
@@ -9040,8 +9040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9057BAD-8FBC-4D49-B900-AD9D698F52D5}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9892,8 +9892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DFAEB1-B984-4ECE-B7FF-70A9C3A4618A}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -10746,7 +10746,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11595,8 +11595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F55ABFB-14F1-408C-BBDD-4655732396A2}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12444,18 +12444,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12649,25 +12649,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B438D6D-30B2-4C3B-929E-B01871068A79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C131489-7CCA-4670-8B56-C6A51A0F0CAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="af16c2e8-b6bd-4b6b-b669-c2f78501a31f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C131489-7CCA-4670-8B56-C6A51A0F0CAB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B438D6D-30B2-4C3B-929E-B01871068A79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="af16c2e8-b6bd-4b6b-b669-c2f78501a31f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>